<commit_message>
added all funtin, no style
</commit_message>
<xml_diff>
--- a/src/Sorce/balanceDP.xlsx
+++ b/src/Sorce/balanceDP.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/SharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="387">
   <si>
     <t>Формирвоание отчета</t>
   </si>
   <si>
-    <t>Период: на 17.01.2025 10:45:11</t>
+    <t>Период: на 20.01.2025 10:55:11</t>
   </si>
   <si>
     <t>Показатели: Свободный остаток(В ед. хранения);</t>
@@ -68,12 +68,18 @@
     <t>Желе апельсин УБ 78г /56шт АКЦІЯ Цінова</t>
   </si>
   <si>
+    <t>Желе вишня УБ 78г /56шт</t>
+  </si>
+  <si>
     <t>Желе ківі УБ 78г /56шт</t>
   </si>
   <si>
     <t>Желе ківі УБ 78г /56шт АКЦІЯ Цінова</t>
   </si>
   <si>
+    <t>Желе Лісова ягода УБ 78г /56шт</t>
+  </si>
+  <si>
     <t>Желе полуниця УБ 78г /56шт</t>
   </si>
   <si>
@@ -200,24 +206,48 @@
     <t>Батон ROSHEN "Double peanuts" мол-шок з арахісом та арахісовим кремом ВКФ 39г /180шт АКЦІЯ ОПТ</t>
   </si>
   <si>
+    <t>Батон ROSHEN "Double peanuts" мол-шок з арахісом та арахісовим кремом ВКФ 39г /180шт ДС</t>
+  </si>
+  <si>
     <t>БАТОН ROSHEN з начинкою 43г/180</t>
   </si>
   <si>
+    <t>Батон ROSHEN з начинкою ВКФ 43г /180шт АКЦІЯ</t>
+  </si>
+  <si>
+    <t>Батон ROSHEN з начинкою ВКФ 43г /180шт ДС</t>
+  </si>
+  <si>
     <t>Батон ROSHEN мол-шок з карамельною начинкою ВКФ 40г /180шт АКЦІЯ ОПТ</t>
   </si>
   <si>
+    <t>Батон ROSHEN мол-шок з карамельною начинкою ВКФ 40г /180шт ДС</t>
+  </si>
+  <si>
     <t>Батон ROSHEN мол-шок з кокосом та мигдалем ВКФ 38г /180шт</t>
   </si>
   <si>
     <t>Батон ROSHEN мол-шок з кокосом та мигдалем ВКФ 38г /180шт АКЦІЯ ОПТ</t>
   </si>
   <si>
+    <t>Батон ROSHEN мол-шок з кокосом та мигдалем ВКФ 38г /180шт ДС</t>
+  </si>
+  <si>
     <t>Батон ROSHEN молочно-шоколадний з арахісовою начинкою ВКФ 38г /180шт</t>
   </si>
   <si>
+    <t>Батон ROSHEN молочно-шоколадний з арахісовою начинкою ВКФ 38г /180шт ДС</t>
+  </si>
+  <si>
     <t>Батон ROSHEN молочно-шоколадний з начинкою крем-брюле ВКФ 43г /180шт АКЦІЯ ОПТ</t>
   </si>
   <si>
+    <t>Батон ROSHEN молочно-шоколадний з начинкою крем-брюле ВКФ 43г /180шт ДС</t>
+  </si>
+  <si>
+    <t>Батон ROSHEN молочно-шоколадний з начинкою крем-брюле ВКФ 43г/180 шт АКЦІЯ</t>
+  </si>
+  <si>
     <t>Батон мол-шок карамель 40г/180/30</t>
   </si>
   <si>
@@ -305,6 +335,9 @@
     <t>Wafers Sandwich Crunch лимон ККФ 142г /15шт /</t>
   </si>
   <si>
+    <t>Wafers Sandwich Crunch полуниця ККФ 142г /15шт /</t>
+  </si>
+  <si>
     <t>Wafers горіх ВКФ 216г /16шт</t>
   </si>
   <si>
@@ -389,6 +422,9 @@
     <t>Yummi Gummi Carrot Farm ВКФ 70г /22шт АКЦІЯ ОПТ</t>
   </si>
   <si>
+    <t>Yummi Gummi Carrots ВКФ 70г /22шт</t>
+  </si>
+  <si>
     <t>Yummi Gummi Cheesecakes ВКФ 70г /22шт</t>
   </si>
   <si>
@@ -740,6 +776,9 @@
     <t>Lovita Jelly Cookies з желейною начинкою зі смаком полуниці ККФ 420г /7шт</t>
   </si>
   <si>
+    <t>Lovita Soft Cream Cookies cocoa ККФ 127г /18шт</t>
+  </si>
+  <si>
     <t>Lovita Soft Cream Cookies hazelnut ККФ 127г /18шт</t>
   </si>
   <si>
@@ -813,9 +852,6 @@
   </si>
   <si>
     <t>Hola! Granola РЦ 0.5кг /8пак</t>
-  </si>
-  <si>
-    <t>Johnny Krocker choco ВКФ 1кг /4шт /</t>
   </si>
   <si>
     <t>Johnny Krocker choco ВКФ 1кг /4шт PL</t>
@@ -1388,7 +1424,7 @@
     <outlinePr summaryBelow="false" summaryRight="false"/>
     <pageSetUpPr autoPageBreaks="false"/>
   </sheetPr>
-  <dimension ref="C375"/>
+  <dimension ref="C387"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -1464,7 +1500,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="12" t="n">
-        <v>648621</v>
+        <v>659343</v>
       </c>
     </row>
     <row r="13" ht="11" customHeight="true" outlineLevel="1">
@@ -1472,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>102505</v>
+        <v>159585</v>
       </c>
     </row>
     <row r="14" ht="11" customHeight="true" outlineLevel="2">
@@ -1480,7 +1516,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>8365</v>
+        <v>15528</v>
       </c>
     </row>
     <row r="15" ht="11" customHeight="true" outlineLevel="3">
@@ -1488,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="16" t="n">
-        <v>1550</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="16" ht="11" customHeight="true" outlineLevel="3">
@@ -1496,31 +1532,31 @@
         <v>15</v>
       </c>
       <c r="C16" s="16" t="n">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="17" ht="11" customHeight="true" outlineLevel="3">
       <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="16" t="n">
-        <v>1217</v>
+      <c r="C17" s="11" t="n">
+        <v>-3</v>
       </c>
     </row>
     <row r="18" ht="11" customHeight="true" outlineLevel="3">
       <c r="B18" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="11" t="n">
-        <v>1</v>
+      <c r="C18" s="16" t="n">
+        <v>2261</v>
       </c>
     </row>
     <row r="19" ht="11" customHeight="true" outlineLevel="3">
       <c r="B19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="16" t="n">
-        <v>1237</v>
+      <c r="C19" s="11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" ht="11" customHeight="true" outlineLevel="3">
@@ -1528,15 +1564,15 @@
         <v>19</v>
       </c>
       <c r="C20" s="16" t="n">
-        <v>2783</v>
-      </c>
-    </row>
-    <row r="21" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B21" s="14" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+    <row r="21" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="12" t="n">
-        <v>30569</v>
+      <c r="C21" s="11" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="22" ht="11" customHeight="true" outlineLevel="3">
@@ -1544,23 +1580,23 @@
         <v>21</v>
       </c>
       <c r="C22" s="16" t="n">
-        <v>4059</v>
-      </c>
-    </row>
-    <row r="23" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B23" s="15" t="s">
+        <v>4916</v>
+      </c>
+    </row>
+    <row r="23" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="16" t="n">
-        <v>6641</v>
+      <c r="C23" s="12" t="n">
+        <v>70000</v>
       </c>
     </row>
     <row r="24" ht="11" customHeight="true" outlineLevel="3">
       <c r="B24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11" t="n">
-        <v>450</v>
+      <c r="C24" s="16" t="n">
+        <v>10350</v>
       </c>
     </row>
     <row r="25" ht="11" customHeight="true" outlineLevel="3">
@@ -1568,7 +1604,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="16" t="n">
-        <v>13459</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="26" ht="11" customHeight="true" outlineLevel="3">
@@ -1576,7 +1612,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="11" t="n">
-        <v>10</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" ht="11" customHeight="true" outlineLevel="3">
@@ -1584,47 +1620,47 @@
         <v>26</v>
       </c>
       <c r="C27" s="16" t="n">
-        <v>2846</v>
+        <v>10579</v>
       </c>
     </row>
     <row r="28" ht="11" customHeight="true" outlineLevel="3">
       <c r="B28" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="16" t="n">
-        <v>3104</v>
-      </c>
-    </row>
-    <row r="29" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B29" s="14" t="s">
+      <c r="C28" s="11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B29" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="12" t="n">
-        <v>16710</v>
+      <c r="C29" s="16" t="n">
+        <v>2643</v>
       </c>
     </row>
     <row r="30" ht="11" customHeight="true" outlineLevel="3">
       <c r="B30" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="11" t="n">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="31" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B31" s="15" t="s">
+      <c r="C30" s="16" t="n">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="31" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B31" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="11" t="n">
-        <v>967</v>
+      <c r="C31" s="12" t="n">
+        <v>16409</v>
       </c>
     </row>
     <row r="32" ht="11" customHeight="true" outlineLevel="3">
       <c r="B32" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="16" t="n">
-        <v>1386</v>
+      <c r="C32" s="11" t="n">
+        <v>579</v>
       </c>
     </row>
     <row r="33" ht="11" customHeight="true" outlineLevel="3">
@@ -1632,39 +1668,39 @@
         <v>32</v>
       </c>
       <c r="C33" s="11" t="n">
-        <v>751</v>
+        <v>863</v>
       </c>
     </row>
     <row r="34" ht="11" customHeight="true" outlineLevel="3">
       <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="11" t="n">
-        <v>582</v>
+      <c r="C34" s="16" t="n">
+        <v>1296</v>
       </c>
     </row>
     <row r="35" ht="11" customHeight="true" outlineLevel="3">
       <c r="B35" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="16" t="n">
-        <v>1677</v>
+      <c r="C35" s="11" t="n">
+        <v>686</v>
       </c>
     </row>
     <row r="36" ht="11" customHeight="true" outlineLevel="3">
       <c r="B36" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="16" t="n">
-        <v>3442</v>
+      <c r="C36" s="11" t="n">
+        <v>532</v>
       </c>
     </row>
     <row r="37" ht="11" customHeight="true" outlineLevel="3">
       <c r="B37" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="11" t="n">
-        <v>362</v>
+      <c r="C37" s="16" t="n">
+        <v>1612</v>
       </c>
     </row>
     <row r="38" ht="11" customHeight="true" outlineLevel="3">
@@ -1672,15 +1708,15 @@
         <v>37</v>
       </c>
       <c r="C38" s="16" t="n">
-        <v>1201</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="39" ht="11" customHeight="true" outlineLevel="3">
       <c r="B39" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="11" t="n">
-        <v>934</v>
+      <c r="C39" s="16" t="n">
+        <v>1159</v>
       </c>
     </row>
     <row r="40" ht="11" customHeight="true" outlineLevel="3">
@@ -1688,7 +1724,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="16" t="n">
-        <v>1021</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="41" ht="11" customHeight="true" outlineLevel="3">
@@ -1696,47 +1732,47 @@
         <v>40</v>
       </c>
       <c r="C41" s="11" t="n">
-        <v>791</v>
+        <v>721</v>
       </c>
     </row>
     <row r="42" ht="11" customHeight="true" outlineLevel="3">
       <c r="B42" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="16" t="n">
-        <v>2917</v>
-      </c>
-    </row>
-    <row r="43" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B43" s="14" t="s">
+      <c r="C42" s="11" t="n">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="43" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B43" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="12" t="n">
-        <v>46861</v>
+      <c r="C43" s="11" t="n">
+        <v>730</v>
       </c>
     </row>
     <row r="44" ht="11" customHeight="true" outlineLevel="3">
       <c r="B44" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="11" t="n">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="45" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B45" s="15" t="s">
+      <c r="C44" s="16" t="n">
+        <v>2797</v>
+      </c>
+    </row>
+    <row r="45" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B45" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="16" t="n">
-        <v>2573</v>
+      <c r="C45" s="12" t="n">
+        <v>57648</v>
       </c>
     </row>
     <row r="46" ht="11" customHeight="true" outlineLevel="3">
       <c r="B46" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="16" t="n">
-        <v>1565</v>
+      <c r="C46" s="11" t="n">
+        <v>696</v>
       </c>
     </row>
     <row r="47" ht="11" customHeight="true" outlineLevel="3">
@@ -1744,7 +1780,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="16" t="n">
-        <v>1224</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="48" ht="11" customHeight="true" outlineLevel="3">
@@ -1752,7 +1788,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="16" t="n">
-        <v>7775</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="49" ht="11" customHeight="true" outlineLevel="3">
@@ -1760,7 +1796,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="16" t="n">
-        <v>2755</v>
+        <v>2847</v>
       </c>
     </row>
     <row r="50" ht="11" customHeight="true" outlineLevel="3">
@@ -1768,7 +1804,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="16" t="n">
-        <v>3779</v>
+        <v>7440</v>
       </c>
     </row>
     <row r="51" ht="11" customHeight="true" outlineLevel="3">
@@ -1776,7 +1812,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="16" t="n">
-        <v>2238</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="52" ht="11" customHeight="true" outlineLevel="3">
@@ -1784,7 +1820,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="16" t="n">
-        <v>1332</v>
+        <v>2966</v>
       </c>
     </row>
     <row r="53" ht="11" customHeight="true" outlineLevel="3">
@@ -1792,7 +1828,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="16" t="n">
-        <v>5367</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="54" ht="11" customHeight="true" outlineLevel="3">
@@ -1800,7 +1836,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="16" t="n">
-        <v>15654</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="55" ht="11" customHeight="true" outlineLevel="3">
@@ -1808,55 +1844,55 @@
         <v>54</v>
       </c>
       <c r="C55" s="16" t="n">
-        <v>1065</v>
+        <v>5137</v>
       </c>
     </row>
     <row r="56" ht="11" customHeight="true" outlineLevel="3">
       <c r="B56" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="11" t="n">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="57" ht="11" customHeight="true" outlineLevel="1">
-      <c r="B57" s="13" t="s">
+      <c r="C56" s="16" t="n">
+        <v>26384</v>
+      </c>
+    </row>
+    <row r="57" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B57" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="12" t="n">
-        <v>546116</v>
-      </c>
-    </row>
-    <row r="58" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B58" s="14" t="s">
+      <c r="C57" s="16" t="n">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="58" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B58" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="12" t="n">
-        <v>185694</v>
-      </c>
-    </row>
-    <row r="59" ht="22" customHeight="true" outlineLevel="3">
-      <c r="B59" s="15" t="s">
+      <c r="C58" s="11" t="n">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="59" ht="11" customHeight="true" outlineLevel="1">
+      <c r="B59" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="16" t="n">
-        <v>41583</v>
-      </c>
-    </row>
-    <row r="60" ht="22" customHeight="true" outlineLevel="3">
-      <c r="B60" s="15" t="s">
+      <c r="C59" s="12" t="n">
+        <v>499758</v>
+      </c>
+    </row>
+    <row r="60" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B60" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="16" t="n">
-        <v>1620</v>
-      </c>
-    </row>
-    <row r="61" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C60" s="12" t="n">
+        <v>131819</v>
+      </c>
+    </row>
+    <row r="61" ht="22" customHeight="true" outlineLevel="3">
       <c r="B61" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="16" t="n">
-        <v>27093</v>
+        <v>28588</v>
       </c>
     </row>
     <row r="62" ht="22" customHeight="true" outlineLevel="3">
@@ -1867,140 +1903,140 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="63" ht="11" customHeight="true" outlineLevel="3">
+    <row r="63" ht="22" customHeight="true" outlineLevel="3">
       <c r="B63" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C63" s="16" t="n">
-        <v>26674</v>
-      </c>
-    </row>
-    <row r="64" ht="22" customHeight="true" outlineLevel="3">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="64" ht="11" customHeight="true" outlineLevel="3">
       <c r="B64" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C64" s="11" t="n">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="65" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C64" s="16" t="n">
+        <v>3073</v>
+      </c>
+    </row>
+    <row r="65" ht="11" customHeight="true" outlineLevel="3">
       <c r="B65" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C65" s="16" t="n">
-        <v>38351</v>
-      </c>
-    </row>
-    <row r="66" ht="22" customHeight="true" outlineLevel="3">
+        <v>5940</v>
+      </c>
+    </row>
+    <row r="66" ht="11" customHeight="true" outlineLevel="3">
       <c r="B66" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C66" s="11" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="67" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C66" s="16" t="n">
+        <v>5940</v>
+      </c>
+    </row>
+    <row r="67" ht="22" customHeight="true" outlineLevel="3">
       <c r="B67" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C67" s="16" t="n">
-        <v>24230</v>
-      </c>
-    </row>
-    <row r="68" ht="11" customHeight="true" outlineLevel="3">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="68" ht="22" customHeight="true" outlineLevel="3">
       <c r="B68" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="16" t="n">
-        <v>23683</v>
-      </c>
-    </row>
-    <row r="69" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B69" s="14" t="s">
+        <v>10980</v>
+      </c>
+    </row>
+    <row r="69" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B69" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="12" t="n">
-        <v>3958</v>
-      </c>
-    </row>
-    <row r="70" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C69" s="16" t="n">
+        <v>13169</v>
+      </c>
+    </row>
+    <row r="70" ht="22" customHeight="true" outlineLevel="3">
       <c r="B70" s="15" t="s">
         <v>69</v>
       </c>
       <c r="C70" s="11" t="n">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="71" ht="11" customHeight="true" outlineLevel="3">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="71" ht="22" customHeight="true" outlineLevel="3">
       <c r="B71" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="11" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C71" s="16" t="n">
+        <v>6840</v>
+      </c>
+    </row>
+    <row r="72" ht="22" customHeight="true" outlineLevel="3">
       <c r="B72" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="11" t="n">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="73" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C72" s="16" t="n">
+        <v>18076</v>
+      </c>
+    </row>
+    <row r="73" ht="22" customHeight="true" outlineLevel="3">
       <c r="B73" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="11" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C73" s="16" t="n">
+        <v>10980</v>
+      </c>
+    </row>
+    <row r="74" ht="22" customHeight="true" outlineLevel="3">
       <c r="B74" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="16" t="n">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="75" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C74" s="11" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" ht="22" customHeight="true" outlineLevel="3">
       <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="11" t="n">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="76" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C75" s="16" t="n">
+        <v>5940</v>
+      </c>
+    </row>
+    <row r="76" ht="22" customHeight="true" outlineLevel="3">
       <c r="B76" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="11" t="n">
-        <v>24</v>
+      <c r="C76" s="16" t="n">
+        <v>5940</v>
       </c>
     </row>
     <row r="77" ht="11" customHeight="true" outlineLevel="3">
       <c r="B77" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="11" t="n">
-        <v>221</v>
+      <c r="C77" s="16" t="n">
+        <v>4030</v>
       </c>
     </row>
     <row r="78" ht="11" customHeight="true" outlineLevel="3">
       <c r="B78" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="11" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B79" s="15" t="s">
+      <c r="C78" s="16" t="n">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="79" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B79" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="11" t="n">
-        <v>155</v>
+      <c r="C79" s="12" t="n">
+        <v>6881</v>
       </c>
     </row>
     <row r="80" ht="11" customHeight="true" outlineLevel="3">
@@ -2008,15 +2044,15 @@
         <v>79</v>
       </c>
       <c r="C80" s="11" t="n">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="81" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B81" s="14" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="81" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B81" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C81" s="12" t="n">
-        <v>69484</v>
+      <c r="C81" s="11" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="82" ht="11" customHeight="true" outlineLevel="3">
@@ -2024,7 +2060,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>181</v>
+        <v>464</v>
       </c>
     </row>
     <row r="83" ht="11" customHeight="true" outlineLevel="3">
@@ -2032,15 +2068,15 @@
         <v>82</v>
       </c>
       <c r="C83" s="11" t="n">
-        <v>709</v>
+        <v>677</v>
       </c>
     </row>
     <row r="84" ht="11" customHeight="true" outlineLevel="3">
       <c r="B84" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C84" s="11" t="n">
-        <v>136</v>
+      <c r="C84" s="16" t="n">
+        <v>1631</v>
       </c>
     </row>
     <row r="85" ht="11" customHeight="true" outlineLevel="3">
@@ -2048,7 +2084,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="11" t="n">
-        <v>91</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" ht="11" customHeight="true" outlineLevel="3">
@@ -2056,47 +2092,47 @@
         <v>85</v>
       </c>
       <c r="C86" s="11" t="n">
-        <v>577</v>
+        <v>865</v>
       </c>
     </row>
     <row r="87" ht="11" customHeight="true" outlineLevel="3">
       <c r="B87" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C87" s="11" t="n">
-        <v>812</v>
+      <c r="C87" s="16" t="n">
+        <v>1141</v>
       </c>
     </row>
     <row r="88" ht="11" customHeight="true" outlineLevel="3">
       <c r="B88" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C88" s="16" t="n">
-        <v>14706</v>
+      <c r="C88" s="11" t="n">
+        <v>308</v>
       </c>
     </row>
     <row r="89" ht="11" customHeight="true" outlineLevel="3">
       <c r="B89" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="16" t="n">
-        <v>26161</v>
+      <c r="C89" s="11" t="n">
+        <v>320</v>
       </c>
     </row>
     <row r="90" ht="11" customHeight="true" outlineLevel="3">
       <c r="B90" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C90" s="16" t="n">
-        <v>17327</v>
-      </c>
-    </row>
-    <row r="91" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B91" s="15" t="s">
+      <c r="C90" s="11" t="n">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B91" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C91" s="11" t="n">
-        <v>250</v>
+      <c r="C91" s="12" t="n">
+        <v>67850</v>
       </c>
     </row>
     <row r="92" ht="11" customHeight="true" outlineLevel="3">
@@ -2104,7 +2140,7 @@
         <v>91</v>
       </c>
       <c r="C92" s="11" t="n">
-        <v>91</v>
+        <v>538</v>
       </c>
     </row>
     <row r="93" ht="11" customHeight="true" outlineLevel="3">
@@ -2112,7 +2148,7 @@
         <v>92</v>
       </c>
       <c r="C93" s="11" t="n">
-        <v>323</v>
+        <v>691</v>
       </c>
     </row>
     <row r="94" ht="11" customHeight="true" outlineLevel="3">
@@ -2120,7 +2156,7 @@
         <v>93</v>
       </c>
       <c r="C94" s="11" t="n">
-        <v>147</v>
+        <v>716</v>
       </c>
     </row>
     <row r="95" ht="11" customHeight="true" outlineLevel="3">
@@ -2128,7 +2164,7 @@
         <v>94</v>
       </c>
       <c r="C95" s="11" t="n">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" ht="11" customHeight="true" outlineLevel="3">
@@ -2136,7 +2172,7 @@
         <v>95</v>
       </c>
       <c r="C96" s="11" t="n">
-        <v>324</v>
+        <v>547</v>
       </c>
     </row>
     <row r="97" ht="11" customHeight="true" outlineLevel="3">
@@ -2144,15 +2180,15 @@
         <v>96</v>
       </c>
       <c r="C97" s="16" t="n">
-        <v>1361</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="98" ht="11" customHeight="true" outlineLevel="3">
       <c r="B98" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="C98" s="11" t="n">
-        <v>138</v>
+      <c r="C98" s="16" t="n">
+        <v>12381</v>
       </c>
     </row>
     <row r="99" ht="11" customHeight="true" outlineLevel="3">
@@ -2160,15 +2196,15 @@
         <v>98</v>
       </c>
       <c r="C99" s="16" t="n">
-        <v>1534</v>
+        <v>25736</v>
       </c>
     </row>
     <row r="100" ht="11" customHeight="true" outlineLevel="3">
       <c r="B100" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="11" t="n">
-        <v>182</v>
+      <c r="C100" s="16" t="n">
+        <v>16077</v>
       </c>
     </row>
     <row r="101" ht="11" customHeight="true" outlineLevel="3">
@@ -2176,7 +2212,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="11" t="n">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="102" ht="11" customHeight="true" outlineLevel="3">
@@ -2184,7 +2220,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="11" t="n">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" ht="11" customHeight="true" outlineLevel="3">
@@ -2192,7 +2228,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="11" t="n">
-        <v>677</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" ht="11" customHeight="true" outlineLevel="3">
@@ -2200,7 +2236,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="11" t="n">
-        <v>561</v>
+        <v>324</v>
       </c>
     </row>
     <row r="105" ht="11" customHeight="true" outlineLevel="3">
@@ -2208,7 +2244,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="11" t="n">
-        <v>660</v>
+        <v>16</v>
       </c>
     </row>
     <row r="106" ht="11" customHeight="true" outlineLevel="3">
@@ -2216,39 +2252,39 @@
         <v>105</v>
       </c>
       <c r="C106" s="11" t="n">
-        <v>91</v>
+        <v>630</v>
       </c>
     </row>
     <row r="107" ht="11" customHeight="true" outlineLevel="3">
       <c r="B107" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C107" s="16" t="n">
-        <v>1016</v>
+      <c r="C107" s="11" t="n">
+        <v>516</v>
       </c>
     </row>
     <row r="108" ht="11" customHeight="true" outlineLevel="3">
       <c r="B108" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C108" s="11" t="n">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="109" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B109" s="14" t="s">
+      <c r="C108" s="16" t="n">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="109" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B109" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C109" s="12" t="n">
-        <v>48322</v>
+      <c r="C109" s="11" t="n">
+        <v>138</v>
       </c>
     </row>
     <row r="110" ht="11" customHeight="true" outlineLevel="3">
       <c r="B110" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C110" s="11" t="n">
-        <v>527</v>
+      <c r="C110" s="16" t="n">
+        <v>1048</v>
       </c>
     </row>
     <row r="111" ht="11" customHeight="true" outlineLevel="3">
@@ -2256,7 +2292,7 @@
         <v>110</v>
       </c>
       <c r="C111" s="11" t="n">
-        <v>576</v>
+        <v>608</v>
       </c>
     </row>
     <row r="112" ht="11" customHeight="true" outlineLevel="3">
@@ -2264,7 +2300,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="11" t="n">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="113" ht="11" customHeight="true" outlineLevel="3">
@@ -2272,15 +2308,15 @@
         <v>112</v>
       </c>
       <c r="C113" s="11" t="n">
-        <v>479</v>
+        <v>436</v>
       </c>
     </row>
     <row r="114" ht="11" customHeight="true" outlineLevel="3">
       <c r="B114" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="C114" s="16" t="n">
-        <v>1690</v>
+      <c r="C114" s="11" t="n">
+        <v>628</v>
       </c>
     </row>
     <row r="115" ht="11" customHeight="true" outlineLevel="3">
@@ -2288,15 +2324,15 @@
         <v>114</v>
       </c>
       <c r="C115" s="11" t="n">
-        <v>428</v>
+        <v>510</v>
       </c>
     </row>
     <row r="116" ht="11" customHeight="true" outlineLevel="3">
       <c r="B116" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C116" s="11" t="n">
-        <v>453</v>
+      <c r="C116" s="16" t="n">
+        <v>1083</v>
       </c>
     </row>
     <row r="117" ht="11" customHeight="true" outlineLevel="3">
@@ -2304,7 +2340,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="11" t="n">
-        <v>350</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118" ht="11" customHeight="true" outlineLevel="3">
@@ -2312,7 +2348,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="11" t="n">
-        <v>134</v>
+        <v>800</v>
       </c>
     </row>
     <row r="119" ht="11" customHeight="true" outlineLevel="3">
@@ -2320,15 +2356,15 @@
         <v>118</v>
       </c>
       <c r="C119" s="11" t="n">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="120" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B120" s="15" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="120" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B120" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C120" s="16" t="n">
-        <v>2176</v>
+      <c r="C120" s="12" t="n">
+        <v>61060</v>
       </c>
     </row>
     <row r="121" ht="11" customHeight="true" outlineLevel="3">
@@ -2336,15 +2372,15 @@
         <v>120</v>
       </c>
       <c r="C121" s="11" t="n">
-        <v>21</v>
+        <v>522</v>
       </c>
     </row>
     <row r="122" ht="11" customHeight="true" outlineLevel="3">
       <c r="B122" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="16" t="n">
-        <v>2176</v>
+      <c r="C122" s="11" t="n">
+        <v>565</v>
       </c>
     </row>
     <row r="123" ht="11" customHeight="true" outlineLevel="3">
@@ -2352,15 +2388,15 @@
         <v>122</v>
       </c>
       <c r="C123" s="11" t="n">
-        <v>8</v>
+        <v>607</v>
       </c>
     </row>
     <row r="124" ht="11" customHeight="true" outlineLevel="3">
       <c r="B124" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="C124" s="16" t="n">
-        <v>1152</v>
+      <c r="C124" s="11" t="n">
+        <v>466</v>
       </c>
     </row>
     <row r="125" ht="11" customHeight="true" outlineLevel="3">
@@ -2368,7 +2404,7 @@
         <v>124</v>
       </c>
       <c r="C125" s="16" t="n">
-        <v>1814</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="126" ht="11" customHeight="true" outlineLevel="3">
@@ -2376,7 +2412,7 @@
         <v>125</v>
       </c>
       <c r="C126" s="11" t="n">
-        <v>19</v>
+        <v>418</v>
       </c>
     </row>
     <row r="127" ht="11" customHeight="true" outlineLevel="3">
@@ -2384,15 +2420,15 @@
         <v>126</v>
       </c>
       <c r="C127" s="11" t="n">
-        <v>14</v>
+        <v>443</v>
       </c>
     </row>
     <row r="128" ht="11" customHeight="true" outlineLevel="3">
       <c r="B128" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="C128" s="16" t="n">
-        <v>1814</v>
+      <c r="C128" s="11" t="n">
+        <v>581</v>
       </c>
     </row>
     <row r="129" ht="11" customHeight="true" outlineLevel="3">
@@ -2400,23 +2436,23 @@
         <v>128</v>
       </c>
       <c r="C129" s="11" t="n">
-        <v>6</v>
+        <v>607</v>
       </c>
     </row>
     <row r="130" ht="11" customHeight="true" outlineLevel="3">
       <c r="B130" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C130" s="11" t="n">
-        <v>693</v>
+      <c r="C130" s="16" t="n">
+        <v>2005</v>
       </c>
     </row>
     <row r="131" ht="11" customHeight="true" outlineLevel="3">
       <c r="B131" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C131" s="11" t="n">
-        <v>724</v>
+      <c r="C131" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="132" ht="11" customHeight="true" outlineLevel="3">
@@ -2424,7 +2460,7 @@
         <v>131</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>625</v>
+        <v>21</v>
       </c>
     </row>
     <row r="133" ht="11" customHeight="true" outlineLevel="3">
@@ -2432,7 +2468,7 @@
         <v>132</v>
       </c>
       <c r="C133" s="16" t="n">
-        <v>1086</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="134" ht="11" customHeight="true" outlineLevel="3">
@@ -2440,23 +2476,23 @@
         <v>133</v>
       </c>
       <c r="C134" s="11" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="135" ht="11" customHeight="true" outlineLevel="3">
       <c r="B135" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="C135" s="11" t="n">
-        <v>724</v>
+      <c r="C135" s="16" t="n">
+        <v>1087</v>
       </c>
     </row>
     <row r="136" ht="11" customHeight="true" outlineLevel="3">
       <c r="B136" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C136" s="11" t="n">
-        <v>283</v>
+      <c r="C136" s="16" t="n">
+        <v>2072</v>
       </c>
     </row>
     <row r="137" ht="11" customHeight="true" outlineLevel="3">
@@ -2464,7 +2500,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="16" t="n">
-        <v>2176</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="138" ht="11" customHeight="true" outlineLevel="3">
@@ -2472,7 +2508,7 @@
         <v>137</v>
       </c>
       <c r="C138" s="11" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="139" ht="11" customHeight="true" outlineLevel="3">
@@ -2480,15 +2516,15 @@
         <v>138</v>
       </c>
       <c r="C139" s="11" t="n">
-        <v>854</v>
+        <v>402</v>
       </c>
     </row>
     <row r="140" ht="11" customHeight="true" outlineLevel="3">
       <c r="B140" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C140" s="11" t="n">
-        <v>724</v>
+      <c r="C140" s="16" t="n">
+        <v>1642</v>
       </c>
     </row>
     <row r="141" ht="11" customHeight="true" outlineLevel="3">
@@ -2496,7 +2532,7 @@
         <v>140</v>
       </c>
       <c r="C141" s="11" t="n">
-        <v>337</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" ht="11" customHeight="true" outlineLevel="3">
@@ -2504,7 +2540,7 @@
         <v>141</v>
       </c>
       <c r="C142" s="16" t="n">
-        <v>2176</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="143" ht="11" customHeight="true" outlineLevel="3">
@@ -2512,15 +2548,15 @@
         <v>142</v>
       </c>
       <c r="C143" s="11" t="n">
-        <v>35</v>
+        <v>660</v>
       </c>
     </row>
     <row r="144" ht="11" customHeight="true" outlineLevel="3">
       <c r="B144" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C144" s="11" t="n">
-        <v>974</v>
+      <c r="C144" s="16" t="n">
+        <v>1002</v>
       </c>
     </row>
     <row r="145" ht="11" customHeight="true" outlineLevel="3">
@@ -2528,7 +2564,7 @@
         <v>144</v>
       </c>
       <c r="C145" s="11" t="n">
-        <v>724</v>
+        <v>990</v>
       </c>
     </row>
     <row r="146" ht="11" customHeight="true" outlineLevel="3">
@@ -2536,47 +2572,47 @@
         <v>145</v>
       </c>
       <c r="C146" s="11" t="n">
-        <v>822</v>
+        <v>788</v>
       </c>
     </row>
     <row r="147" ht="11" customHeight="true" outlineLevel="3">
       <c r="B147" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C147" s="16" t="n">
-        <v>2176</v>
+      <c r="C147" s="11" t="n">
+        <v>660</v>
       </c>
     </row>
     <row r="148" ht="11" customHeight="true" outlineLevel="3">
       <c r="B148" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C148" s="11" t="n">
-        <v>507</v>
+      <c r="C148" s="16" t="n">
+        <v>1343</v>
       </c>
     </row>
     <row r="149" ht="11" customHeight="true" outlineLevel="3">
       <c r="B149" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C149" s="11" t="n">
-        <v>658</v>
+      <c r="C149" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="150" ht="11" customHeight="true" outlineLevel="3">
       <c r="B150" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C150" s="16" t="n">
-        <v>1086</v>
+      <c r="C150" s="11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="151" ht="11" customHeight="true" outlineLevel="3">
       <c r="B151" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C151" s="11" t="n">
-        <v>164</v>
+      <c r="C151" s="16" t="n">
+        <v>1174</v>
       </c>
     </row>
     <row r="152" ht="11" customHeight="true" outlineLevel="3">
@@ -2584,31 +2620,31 @@
         <v>151</v>
       </c>
       <c r="C152" s="11" t="n">
-        <v>724</v>
+        <v>660</v>
       </c>
     </row>
     <row r="153" ht="11" customHeight="true" outlineLevel="3">
       <c r="B153" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="C153" s="11" t="n">
-        <v>125</v>
+      <c r="C153" s="16" t="n">
+        <v>1395</v>
       </c>
     </row>
     <row r="154" ht="11" customHeight="true" outlineLevel="3">
       <c r="B154" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C154" s="11" t="n">
-        <v>700</v>
+      <c r="C154" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="155" ht="11" customHeight="true" outlineLevel="3">
       <c r="B155" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="C155" s="16" t="n">
-        <v>2176</v>
+      <c r="C155" s="11" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="156" ht="11" customHeight="true" outlineLevel="3">
@@ -2616,7 +2652,7 @@
         <v>155</v>
       </c>
       <c r="C156" s="11" t="n">
-        <v>308</v>
+        <v>730</v>
       </c>
     </row>
     <row r="157" ht="11" customHeight="true" outlineLevel="3">
@@ -2624,7 +2660,7 @@
         <v>156</v>
       </c>
       <c r="C157" s="11" t="n">
-        <v>456</v>
+        <v>660</v>
       </c>
     </row>
     <row r="158" ht="11" customHeight="true" outlineLevel="3">
@@ -2632,15 +2668,15 @@
         <v>157</v>
       </c>
       <c r="C158" s="16" t="n">
-        <v>1086</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="159" ht="11" customHeight="true" outlineLevel="3">
       <c r="B159" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C159" s="11" t="n">
-        <v>220</v>
+      <c r="C159" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="160" ht="11" customHeight="true" outlineLevel="3">
@@ -2648,15 +2684,15 @@
         <v>159</v>
       </c>
       <c r="C160" s="11" t="n">
-        <v>86</v>
+        <v>507</v>
       </c>
     </row>
     <row r="161" ht="11" customHeight="true" outlineLevel="3">
       <c r="B161" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C161" s="16" t="n">
-        <v>2176</v>
+      <c r="C161" s="11" t="n">
+        <v>913</v>
       </c>
     </row>
     <row r="162" ht="11" customHeight="true" outlineLevel="3">
@@ -2664,7 +2700,7 @@
         <v>161</v>
       </c>
       <c r="C162" s="11" t="n">
-        <v>734</v>
+        <v>990</v>
       </c>
     </row>
     <row r="163" ht="11" customHeight="true" outlineLevel="3">
@@ -2672,7 +2708,7 @@
         <v>162</v>
       </c>
       <c r="C163" s="11" t="n">
-        <v>724</v>
+        <v>477</v>
       </c>
     </row>
     <row r="164" ht="11" customHeight="true" outlineLevel="3">
@@ -2680,39 +2716,39 @@
         <v>163</v>
       </c>
       <c r="C164" s="11" t="n">
-        <v>10</v>
+        <v>660</v>
       </c>
     </row>
     <row r="165" ht="11" customHeight="true" outlineLevel="3">
       <c r="B165" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="C165" s="16" t="n">
-        <v>1814</v>
+      <c r="C165" s="11" t="n">
+        <v>125</v>
       </c>
     </row>
     <row r="166" ht="11" customHeight="true" outlineLevel="3">
       <c r="B166" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="C166" s="11" t="n">
-        <v>176</v>
+      <c r="C166" s="16" t="n">
+        <v>1567</v>
       </c>
     </row>
     <row r="167" ht="11" customHeight="true" outlineLevel="3">
       <c r="B167" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C167" s="11" t="n">
-        <v>30</v>
+      <c r="C167" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="168" ht="11" customHeight="true" outlineLevel="3">
       <c r="B168" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="C168" s="16" t="n">
-        <v>1053</v>
+      <c r="C168" s="11" t="n">
+        <v>308</v>
       </c>
     </row>
     <row r="169" ht="11" customHeight="true" outlineLevel="3">
@@ -2720,7 +2756,7 @@
         <v>168</v>
       </c>
       <c r="C169" s="11" t="n">
-        <v>100</v>
+        <v>938</v>
       </c>
     </row>
     <row r="170" ht="11" customHeight="true" outlineLevel="3">
@@ -2728,7 +2764,7 @@
         <v>169</v>
       </c>
       <c r="C170" s="11" t="n">
-        <v>612</v>
+        <v>990</v>
       </c>
     </row>
     <row r="171" ht="11" customHeight="true" outlineLevel="3">
@@ -2736,31 +2772,31 @@
         <v>170</v>
       </c>
       <c r="C171" s="11" t="n">
-        <v>840</v>
+        <v>220</v>
       </c>
     </row>
     <row r="172" ht="11" customHeight="true" outlineLevel="3">
       <c r="B172" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C172" s="11" t="n">
-        <v>578</v>
+      <c r="C172" s="16" t="n">
+        <v>1156</v>
       </c>
     </row>
     <row r="173" ht="11" customHeight="true" outlineLevel="3">
       <c r="B173" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C173" s="11" t="n">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="174" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B174" s="14" t="s">
+      <c r="C173" s="16" t="n">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="174" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B174" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="C174" s="12" t="n">
-        <v>42749</v>
+      <c r="C174" s="16" t="n">
+        <v>1008</v>
       </c>
     </row>
     <row r="175" ht="11" customHeight="true" outlineLevel="3">
@@ -2768,31 +2804,31 @@
         <v>174</v>
       </c>
       <c r="C175" s="11" t="n">
-        <v>735</v>
+        <v>660</v>
       </c>
     </row>
     <row r="176" ht="11" customHeight="true" outlineLevel="3">
       <c r="B176" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C176" s="16" t="n">
-        <v>1705</v>
+      <c r="C176" s="11" t="n">
+        <v>923</v>
       </c>
     </row>
     <row r="177" ht="11" customHeight="true" outlineLevel="3">
       <c r="B177" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C177" s="11" t="n">
-        <v>635</v>
+      <c r="C177" s="16" t="n">
+        <v>1642</v>
       </c>
     </row>
     <row r="178" ht="11" customHeight="true" outlineLevel="3">
       <c r="B178" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C178" s="16" t="n">
-        <v>2717</v>
+      <c r="C178" s="11" t="n">
+        <v>176</v>
       </c>
     </row>
     <row r="179" ht="11" customHeight="true" outlineLevel="3">
@@ -2800,23 +2836,23 @@
         <v>178</v>
       </c>
       <c r="C179" s="11" t="n">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="180" ht="11" customHeight="true" outlineLevel="3">
       <c r="B180" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="C180" s="11" t="n">
-        <v>96</v>
+      <c r="C180" s="16" t="n">
+        <v>1052</v>
       </c>
     </row>
     <row r="181" ht="11" customHeight="true" outlineLevel="3">
       <c r="B181" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="C181" s="11" t="n">
-        <v>199</v>
+      <c r="C181" s="16" t="n">
+        <v>1208</v>
       </c>
     </row>
     <row r="182" ht="11" customHeight="true" outlineLevel="3">
@@ -2824,7 +2860,7 @@
         <v>181</v>
       </c>
       <c r="C182" s="11" t="n">
-        <v>823</v>
+        <v>607</v>
       </c>
     </row>
     <row r="183" ht="11" customHeight="true" outlineLevel="3">
@@ -2832,15 +2868,15 @@
         <v>182</v>
       </c>
       <c r="C183" s="11" t="n">
-        <v>918</v>
+        <v>840</v>
       </c>
     </row>
     <row r="184" ht="11" customHeight="true" outlineLevel="3">
       <c r="B184" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="C184" s="16" t="n">
-        <v>1009</v>
+      <c r="C184" s="11" t="n">
+        <v>542</v>
       </c>
     </row>
     <row r="185" ht="11" customHeight="true" outlineLevel="3">
@@ -2848,15 +2884,15 @@
         <v>184</v>
       </c>
       <c r="C185" s="16" t="n">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="186" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B186" s="15" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="186" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B186" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C186" s="16" t="n">
-        <v>1103</v>
+      <c r="C186" s="12" t="n">
+        <v>43315</v>
       </c>
     </row>
     <row r="187" ht="11" customHeight="true" outlineLevel="3">
@@ -2864,7 +2900,7 @@
         <v>186</v>
       </c>
       <c r="C187" s="16" t="n">
-        <v>1038</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="188" ht="11" customHeight="true" outlineLevel="3">
@@ -2872,15 +2908,15 @@
         <v>187</v>
       </c>
       <c r="C188" s="16" t="n">
-        <v>1190</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="189" ht="11" customHeight="true" outlineLevel="3">
       <c r="B189" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C189" s="11" t="n">
-        <v>388</v>
+      <c r="C189" s="16" t="n">
+        <v>1137</v>
       </c>
     </row>
     <row r="190" ht="11" customHeight="true" outlineLevel="3">
@@ -2888,7 +2924,7 @@
         <v>189</v>
       </c>
       <c r="C190" s="16" t="n">
-        <v>1175</v>
+        <v>3338</v>
       </c>
     </row>
     <row r="191" ht="11" customHeight="true" outlineLevel="3">
@@ -2896,7 +2932,7 @@
         <v>190</v>
       </c>
       <c r="C191" s="11" t="n">
-        <v>952</v>
+        <v>44</v>
       </c>
     </row>
     <row r="192" ht="11" customHeight="true" outlineLevel="3">
@@ -2904,31 +2940,31 @@
         <v>191</v>
       </c>
       <c r="C192" s="11" t="n">
-        <v>897</v>
+        <v>238</v>
       </c>
     </row>
     <row r="193" ht="11" customHeight="true" outlineLevel="3">
       <c r="B193" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C193" s="16" t="n">
-        <v>1572</v>
+      <c r="C193" s="11" t="n">
+        <v>330</v>
       </c>
     </row>
     <row r="194" ht="11" customHeight="true" outlineLevel="3">
       <c r="B194" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="C194" s="16" t="n">
-        <v>1667</v>
+      <c r="C194" s="11" t="n">
+        <v>764</v>
       </c>
     </row>
     <row r="195" ht="11" customHeight="true" outlineLevel="3">
       <c r="B195" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C195" s="16" t="n">
-        <v>2646</v>
+      <c r="C195" s="11" t="n">
+        <v>886</v>
       </c>
     </row>
     <row r="196" ht="11" customHeight="true" outlineLevel="3">
@@ -2936,7 +2972,7 @@
         <v>195</v>
       </c>
       <c r="C196" s="16" t="n">
-        <v>2379</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="197" ht="11" customHeight="true" outlineLevel="3">
@@ -2944,7 +2980,7 @@
         <v>196</v>
       </c>
       <c r="C197" s="16" t="n">
-        <v>2260</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="198" ht="11" customHeight="true" outlineLevel="3">
@@ -2952,15 +2988,15 @@
         <v>197</v>
       </c>
       <c r="C198" s="16" t="n">
-        <v>1842</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="199" ht="11" customHeight="true" outlineLevel="3">
       <c r="B199" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C199" s="11" t="n">
-        <v>213</v>
+      <c r="C199" s="16" t="n">
+        <v>1017</v>
       </c>
     </row>
     <row r="200" ht="11" customHeight="true" outlineLevel="3">
@@ -2968,15 +3004,15 @@
         <v>199</v>
       </c>
       <c r="C200" s="16" t="n">
-        <v>2355</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="201" ht="11" customHeight="true" outlineLevel="3">
       <c r="B201" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C201" s="16" t="n">
-        <v>2018</v>
+      <c r="C201" s="11" t="n">
+        <v>355</v>
       </c>
     </row>
     <row r="202" ht="11" customHeight="true" outlineLevel="3">
@@ -2984,23 +3020,23 @@
         <v>201</v>
       </c>
       <c r="C202" s="16" t="n">
-        <v>1267</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="203" ht="11" customHeight="true" outlineLevel="3">
       <c r="B203" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="C203" s="16" t="n">
-        <v>2242</v>
+      <c r="C203" s="11" t="n">
+        <v>889</v>
       </c>
     </row>
     <row r="204" ht="11" customHeight="true" outlineLevel="3">
       <c r="B204" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="C204" s="16" t="n">
-        <v>1824</v>
+      <c r="C204" s="11" t="n">
+        <v>864</v>
       </c>
     </row>
     <row r="205" ht="11" customHeight="true" outlineLevel="3">
@@ -3008,47 +3044,47 @@
         <v>204</v>
       </c>
       <c r="C205" s="16" t="n">
-        <v>2727</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="206" ht="11" customHeight="true" outlineLevel="3">
       <c r="B206" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="C206" s="11" t="n">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="207" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B207" s="14" t="s">
+      <c r="C206" s="16" t="n">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="207" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B207" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C207" s="12" t="n">
-        <v>5460</v>
+      <c r="C207" s="16" t="n">
+        <v>2475</v>
       </c>
     </row>
     <row r="208" ht="11" customHeight="true" outlineLevel="3">
       <c r="B208" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C208" s="11" t="n">
-        <v>340</v>
+      <c r="C208" s="16" t="n">
+        <v>2260</v>
       </c>
     </row>
     <row r="209" ht="11" customHeight="true" outlineLevel="3">
       <c r="B209" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="C209" s="11" t="n">
-        <v>26</v>
+      <c r="C209" s="16" t="n">
+        <v>1984</v>
       </c>
     </row>
     <row r="210" ht="11" customHeight="true" outlineLevel="3">
       <c r="B210" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="C210" s="11" t="n">
-        <v>993</v>
+      <c r="C210" s="16" t="n">
+        <v>2191</v>
       </c>
     </row>
     <row r="211" ht="11" customHeight="true" outlineLevel="3">
@@ -3056,31 +3092,31 @@
         <v>210</v>
       </c>
       <c r="C211" s="11" t="n">
-        <v>192</v>
+        <v>213</v>
       </c>
     </row>
     <row r="212" ht="11" customHeight="true" outlineLevel="3">
       <c r="B212" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="C212" s="11" t="n">
-        <v>338</v>
+      <c r="C212" s="16" t="n">
+        <v>2134</v>
       </c>
     </row>
     <row r="213" ht="11" customHeight="true" outlineLevel="3">
       <c r="B213" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="C213" s="11" t="n">
-        <v>13</v>
+      <c r="C213" s="16" t="n">
+        <v>2444</v>
       </c>
     </row>
     <row r="214" ht="11" customHeight="true" outlineLevel="3">
       <c r="B214" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="C214" s="11" t="n">
-        <v>89</v>
+      <c r="C214" s="16" t="n">
+        <v>1087</v>
       </c>
     </row>
     <row r="215" ht="11" customHeight="true" outlineLevel="3">
@@ -3088,23 +3124,23 @@
         <v>214</v>
       </c>
       <c r="C215" s="16" t="n">
-        <v>1047</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="216" ht="11" customHeight="true" outlineLevel="3">
       <c r="B216" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C216" s="11" t="n">
-        <v>366</v>
+      <c r="C216" s="16" t="n">
+        <v>1734</v>
       </c>
     </row>
     <row r="217" ht="11" customHeight="true" outlineLevel="3">
       <c r="B217" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="C217" s="11" t="n">
-        <v>391</v>
+      <c r="C217" s="16" t="n">
+        <v>3110</v>
       </c>
     </row>
     <row r="218" ht="11" customHeight="true" outlineLevel="3">
@@ -3112,15 +3148,15 @@
         <v>217</v>
       </c>
       <c r="C218" s="11" t="n">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="219" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B219" s="15" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="219" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B219" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="C219" s="11" t="n">
-        <v>384</v>
+      <c r="C219" s="12" t="n">
+        <v>5175</v>
       </c>
     </row>
     <row r="220" ht="11" customHeight="true" outlineLevel="3">
@@ -3128,7 +3164,7 @@
         <v>219</v>
       </c>
       <c r="C220" s="11" t="n">
-        <v>453</v>
+        <v>303</v>
       </c>
     </row>
     <row r="221" ht="11" customHeight="true" outlineLevel="3">
@@ -3136,7 +3172,7 @@
         <v>220</v>
       </c>
       <c r="C221" s="11" t="n">
-        <v>203</v>
+        <v>26</v>
       </c>
     </row>
     <row r="222" ht="11" customHeight="true" outlineLevel="3">
@@ -3144,7 +3180,7 @@
         <v>221</v>
       </c>
       <c r="C222" s="11" t="n">
-        <v>9</v>
+        <v>937</v>
       </c>
     </row>
     <row r="223" ht="11" customHeight="true" outlineLevel="3">
@@ -3152,23 +3188,23 @@
         <v>222</v>
       </c>
       <c r="C223" s="11" t="n">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="224" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B224" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="224" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B224" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C224" s="12" t="n">
-        <v>30089</v>
-      </c>
-    </row>
-    <row r="225" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C224" s="11" t="n">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="225" ht="11" customHeight="true" outlineLevel="3">
       <c r="B225" s="15" t="s">
         <v>224</v>
       </c>
       <c r="C225" s="11" t="n">
-        <v>315</v>
+        <v>13</v>
       </c>
     </row>
     <row r="226" ht="11" customHeight="true" outlineLevel="3">
@@ -3176,15 +3212,15 @@
         <v>225</v>
       </c>
       <c r="C226" s="11" t="n">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="227" ht="11" customHeight="true" outlineLevel="3">
       <c r="B227" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="C227" s="11" t="n">
-        <v>233</v>
+      <c r="C227" s="16" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="228" ht="11" customHeight="true" outlineLevel="3">
@@ -3192,7 +3228,7 @@
         <v>227</v>
       </c>
       <c r="C228" s="11" t="n">
-        <v>500</v>
+        <v>331</v>
       </c>
     </row>
     <row r="229" ht="11" customHeight="true" outlineLevel="3">
@@ -3200,7 +3236,7 @@
         <v>228</v>
       </c>
       <c r="C229" s="11" t="n">
-        <v>755</v>
+        <v>363</v>
       </c>
     </row>
     <row r="230" ht="11" customHeight="true" outlineLevel="3">
@@ -3208,7 +3244,7 @@
         <v>229</v>
       </c>
       <c r="C230" s="11" t="n">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="231" ht="11" customHeight="true" outlineLevel="3">
@@ -3216,47 +3252,47 @@
         <v>230</v>
       </c>
       <c r="C231" s="11" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="232" ht="22" customHeight="true" outlineLevel="3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="232" ht="11" customHeight="true" outlineLevel="3">
       <c r="B232" s="15" t="s">
         <v>231</v>
       </c>
       <c r="C232" s="11" t="n">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="233" ht="22" customHeight="true" outlineLevel="3">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="233" ht="11" customHeight="true" outlineLevel="3">
       <c r="B233" s="15" t="s">
         <v>232</v>
       </c>
       <c r="C233" s="11" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="234" ht="22" customHeight="true" outlineLevel="3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="234" ht="11" customHeight="true" outlineLevel="3">
       <c r="B234" s="15" t="s">
         <v>233</v>
       </c>
       <c r="C234" s="11" t="n">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="235" ht="22" customHeight="true" outlineLevel="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" ht="11" customHeight="true" outlineLevel="3">
       <c r="B235" s="15" t="s">
         <v>234</v>
       </c>
       <c r="C235" s="11" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="236" ht="22" customHeight="true" outlineLevel="3">
-      <c r="B236" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="236" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B236" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="C236" s="11" t="n">
-        <v>24</v>
+      <c r="C236" s="12" t="n">
+        <v>31099</v>
       </c>
     </row>
     <row r="237" ht="22" customHeight="true" outlineLevel="3">
@@ -3264,31 +3300,31 @@
         <v>236</v>
       </c>
       <c r="C237" s="11" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="238" ht="22" customHeight="true" outlineLevel="3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="238" ht="11" customHeight="true" outlineLevel="3">
       <c r="B238" s="15" t="s">
         <v>237</v>
       </c>
       <c r="C238" s="11" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="239" ht="22" customHeight="true" outlineLevel="3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="239" ht="11" customHeight="true" outlineLevel="3">
       <c r="B239" s="15" t="s">
         <v>238</v>
       </c>
       <c r="C239" s="11" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="240" ht="22" customHeight="true" outlineLevel="3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="240" ht="11" customHeight="true" outlineLevel="3">
       <c r="B240" s="15" t="s">
         <v>239</v>
       </c>
       <c r="C240" s="11" t="n">
-        <v>124</v>
+        <v>489</v>
       </c>
     </row>
     <row r="241" ht="11" customHeight="true" outlineLevel="3">
@@ -3296,15 +3332,15 @@
         <v>240</v>
       </c>
       <c r="C241" s="11" t="n">
-        <v>19</v>
+        <v>372</v>
       </c>
     </row>
     <row r="242" ht="11" customHeight="true" outlineLevel="3">
       <c r="B242" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C242" s="11" t="n">
-        <v>91</v>
+      <c r="C242" s="16" t="n">
+        <v>1444</v>
       </c>
     </row>
     <row r="243" ht="11" customHeight="true" outlineLevel="3">
@@ -3312,103 +3348,103 @@
         <v>242</v>
       </c>
       <c r="C243" s="11" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="244" ht="11" customHeight="true" outlineLevel="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="244" ht="22" customHeight="true" outlineLevel="3">
       <c r="B244" s="15" t="s">
         <v>243</v>
       </c>
       <c r="C244" s="11" t="n">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="245" ht="11" customHeight="true" outlineLevel="3">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="245" ht="22" customHeight="true" outlineLevel="3">
       <c r="B245" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C245" s="16" t="n">
-        <v>2889</v>
-      </c>
-    </row>
-    <row r="246" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C245" s="11" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="246" ht="22" customHeight="true" outlineLevel="3">
       <c r="B246" s="15" t="s">
         <v>245</v>
       </c>
       <c r="C246" s="11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="247" ht="11" customHeight="true" outlineLevel="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="247" ht="22" customHeight="true" outlineLevel="3">
       <c r="B247" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C247" s="16" t="n">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="248" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C247" s="11" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="248" ht="22" customHeight="true" outlineLevel="3">
       <c r="B248" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C248" s="16" t="n">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="249" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C248" s="11" t="n">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="249" ht="22" customHeight="true" outlineLevel="3">
       <c r="B249" s="15" t="s">
         <v>248</v>
       </c>
       <c r="C249" s="11" t="n">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="250" ht="11" customHeight="true" outlineLevel="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="250" ht="22" customHeight="true" outlineLevel="3">
       <c r="B250" s="15" t="s">
         <v>249</v>
       </c>
       <c r="C250" s="11" t="n">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="251" ht="11" customHeight="true" outlineLevel="3">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="251" ht="22" customHeight="true" outlineLevel="3">
       <c r="B251" s="15" t="s">
         <v>250</v>
       </c>
       <c r="C251" s="11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="252" ht="11" customHeight="true" outlineLevel="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="252" ht="22" customHeight="true" outlineLevel="3">
       <c r="B252" s="15" t="s">
         <v>251</v>
       </c>
       <c r="C252" s="11" t="n">
-        <v>310</v>
+        <v>119</v>
       </c>
     </row>
     <row r="253" ht="11" customHeight="true" outlineLevel="3">
       <c r="B253" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C253" s="16" t="n">
-        <v>2262</v>
+      <c r="C253" s="11" t="n">
+        <v>379</v>
       </c>
     </row>
     <row r="254" ht="11" customHeight="true" outlineLevel="3">
       <c r="B254" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C254" s="16" t="n">
-        <v>11975</v>
+      <c r="C254" s="11" t="n">
+        <v>401</v>
       </c>
     </row>
     <row r="255" ht="11" customHeight="true" outlineLevel="3">
       <c r="B255" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C255" s="16" t="n">
-        <v>4093</v>
+      <c r="C255" s="11" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="256" ht="11" customHeight="true" outlineLevel="3">
@@ -3416,23 +3452,23 @@
         <v>255</v>
       </c>
       <c r="C256" s="11" t="n">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="257" ht="22" customHeight="true" outlineLevel="3">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="257" ht="11" customHeight="true" outlineLevel="3">
       <c r="B257" s="15" t="s">
         <v>256</v>
       </c>
       <c r="C257" s="11" t="n">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="258" ht="22" customHeight="true" outlineLevel="3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="258" ht="11" customHeight="true" outlineLevel="3">
       <c r="B258" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="C258" s="11" t="n">
-        <v>1</v>
+      <c r="C258" s="16" t="n">
+        <v>2748</v>
       </c>
     </row>
     <row r="259" ht="11" customHeight="true" outlineLevel="3">
@@ -3440,23 +3476,23 @@
         <v>258</v>
       </c>
       <c r="C259" s="11" t="n">
-        <v>242</v>
+        <v>4</v>
       </c>
     </row>
     <row r="260" ht="11" customHeight="true" outlineLevel="3">
       <c r="B260" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="C260" s="11" t="n">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="261" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B261" s="14" t="s">
+      <c r="C260" s="16" t="n">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="261" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B261" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="C261" s="12" t="n">
-        <v>44270</v>
+      <c r="C261" s="16" t="n">
+        <v>2627</v>
       </c>
     </row>
     <row r="262" ht="11" customHeight="true" outlineLevel="3">
@@ -3464,79 +3500,79 @@
         <v>261</v>
       </c>
       <c r="C262" s="16" t="n">
-        <v>2052</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="263" ht="11" customHeight="true" outlineLevel="3">
       <c r="B263" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C263" s="16" t="n">
-        <v>2661</v>
+      <c r="C263" s="11" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="264" ht="11" customHeight="true" outlineLevel="3">
       <c r="B264" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="C264" s="16" t="n">
-        <v>3172</v>
+      <c r="C264" s="11" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="265" ht="11" customHeight="true" outlineLevel="3">
       <c r="B265" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C265" s="16" t="n">
-        <v>1049</v>
+      <c r="C265" s="11" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="266" ht="11" customHeight="true" outlineLevel="3">
       <c r="B266" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="C266" s="11" t="n">
-        <v>14</v>
+      <c r="C266" s="16" t="n">
+        <v>1534</v>
       </c>
     </row>
     <row r="267" ht="11" customHeight="true" outlineLevel="3">
       <c r="B267" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="C267" s="11" t="n">
-        <v>716</v>
+      <c r="C267" s="16" t="n">
+        <v>9042</v>
       </c>
     </row>
     <row r="268" ht="11" customHeight="true" outlineLevel="3">
       <c r="B268" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C268" s="11" t="n">
-        <v>751</v>
+      <c r="C268" s="16" t="n">
+        <v>2830</v>
       </c>
     </row>
     <row r="269" ht="11" customHeight="true" outlineLevel="3">
       <c r="B269" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="C269" s="11" t="n">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="270" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C269" s="16" t="n">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="270" ht="22" customHeight="true" outlineLevel="3">
       <c r="B270" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="C270" s="16" t="n">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="271" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C270" s="11" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="271" ht="22" customHeight="true" outlineLevel="3">
       <c r="B271" s="15" t="s">
         <v>270</v>
       </c>
-      <c r="C271" s="16" t="n">
-        <v>2391</v>
+      <c r="C271" s="11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="272" ht="11" customHeight="true" outlineLevel="3">
@@ -3544,47 +3580,47 @@
         <v>271</v>
       </c>
       <c r="C272" s="11" t="n">
-        <v>557</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" ht="11" customHeight="true" outlineLevel="3">
       <c r="B273" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="C273" s="16" t="n">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="274" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B274" s="15" t="s">
+      <c r="C273" s="11" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="274" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B274" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="C274" s="16" t="n">
-        <v>1278</v>
+      <c r="C274" s="12" t="n">
+        <v>40713</v>
       </c>
     </row>
     <row r="275" ht="11" customHeight="true" outlineLevel="3">
       <c r="B275" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C275" s="11" t="n">
-        <v>403</v>
+      <c r="C275" s="16" t="n">
+        <v>1358</v>
       </c>
     </row>
     <row r="276" ht="11" customHeight="true" outlineLevel="3">
       <c r="B276" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="C276" s="11" t="n">
-        <v>8</v>
+      <c r="C276" s="16" t="n">
+        <v>2289</v>
       </c>
     </row>
     <row r="277" ht="11" customHeight="true" outlineLevel="3">
       <c r="B277" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C277" s="11" t="n">
-        <v>418</v>
+      <c r="C277" s="16" t="n">
+        <v>2658</v>
       </c>
     </row>
     <row r="278" ht="11" customHeight="true" outlineLevel="3">
@@ -3592,23 +3628,23 @@
         <v>277</v>
       </c>
       <c r="C278" s="11" t="n">
-        <v>203</v>
+        <v>975</v>
       </c>
     </row>
     <row r="279" ht="11" customHeight="true" outlineLevel="3">
       <c r="B279" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="C279" s="11" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="280" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C279" s="16" t="n">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="280" ht="11" customHeight="true" outlineLevel="3">
       <c r="B280" s="15" t="s">
         <v>279</v>
       </c>
       <c r="C280" s="11" t="n">
-        <v>236</v>
+        <v>639</v>
       </c>
     </row>
     <row r="281" ht="11" customHeight="true" outlineLevel="3">
@@ -3616,31 +3652,31 @@
         <v>280</v>
       </c>
       <c r="C281" s="11" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="282" ht="22" customHeight="true" outlineLevel="3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="282" ht="11" customHeight="true" outlineLevel="3">
       <c r="B282" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="C282" s="11" t="n">
-        <v>7</v>
+      <c r="C282" s="16" t="n">
+        <v>1416</v>
       </c>
     </row>
     <row r="283" ht="11" customHeight="true" outlineLevel="3">
       <c r="B283" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C283" s="11" t="n">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="284" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C283" s="16" t="n">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="284" ht="11" customHeight="true" outlineLevel="3">
       <c r="B284" s="15" t="s">
         <v>283</v>
       </c>
       <c r="C284" s="11" t="n">
-        <v>294</v>
+        <v>709</v>
       </c>
     </row>
     <row r="285" ht="11" customHeight="true" outlineLevel="3">
@@ -3648,47 +3684,47 @@
         <v>284</v>
       </c>
       <c r="C285" s="16" t="n">
-        <v>13540</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="286" ht="11" customHeight="true" outlineLevel="3">
       <c r="B286" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="C286" s="11" t="n">
-        <v>24</v>
+      <c r="C286" s="16" t="n">
+        <v>1179</v>
       </c>
     </row>
     <row r="287" ht="11" customHeight="true" outlineLevel="3">
       <c r="B287" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="C287" s="16" t="n">
-        <v>7520</v>
+      <c r="C287" s="11" t="n">
+        <v>379</v>
       </c>
     </row>
     <row r="288" ht="11" customHeight="true" outlineLevel="3">
       <c r="B288" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="C288" s="16" t="n">
-        <v>2001</v>
+      <c r="C288" s="11" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="289" ht="11" customHeight="true" outlineLevel="3">
       <c r="B289" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C289" s="16" t="n">
-        <v>1235</v>
-      </c>
-    </row>
-    <row r="290" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B290" s="14" t="s">
+      <c r="C289" s="11" t="n">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="290" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B290" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="C290" s="17" t="n">
-        <v>523</v>
+      <c r="C290" s="11" t="n">
+        <v>175</v>
       </c>
     </row>
     <row r="291" ht="11" customHeight="true" outlineLevel="3">
@@ -3696,15 +3732,15 @@
         <v>290</v>
       </c>
       <c r="C291" s="11" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="292" ht="11" customHeight="true" outlineLevel="3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="292" ht="22" customHeight="true" outlineLevel="3">
       <c r="B292" s="15" t="s">
         <v>291</v>
       </c>
       <c r="C292" s="11" t="n">
-        <v>48</v>
+        <v>235</v>
       </c>
     </row>
     <row r="293" ht="11" customHeight="true" outlineLevel="3">
@@ -3712,103 +3748,103 @@
         <v>292</v>
       </c>
       <c r="C293" s="11" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="294" ht="11" customHeight="true" outlineLevel="3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="294" ht="22" customHeight="true" outlineLevel="3">
       <c r="B294" s="15" t="s">
         <v>293</v>
       </c>
       <c r="C294" s="11" t="n">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="295" ht="11" customHeight="true" outlineLevel="2">
-      <c r="B295" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="295" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B295" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="C295" s="12" t="n">
-        <v>115567</v>
-      </c>
-    </row>
-    <row r="296" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C295" s="11" t="n">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="296" ht="22" customHeight="true" outlineLevel="3">
       <c r="B296" s="15" t="s">
         <v>295</v>
       </c>
       <c r="C296" s="11" t="n">
-        <v>237</v>
+        <v>293</v>
       </c>
     </row>
     <row r="297" ht="11" customHeight="true" outlineLevel="3">
       <c r="B297" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C297" s="11" t="n">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="298" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C297" s="16" t="n">
+        <v>13170</v>
+      </c>
+    </row>
+    <row r="298" ht="11" customHeight="true" outlineLevel="3">
       <c r="B298" s="15" t="s">
         <v>297</v>
       </c>
       <c r="C298" s="11" t="n">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="299" ht="22" customHeight="true" outlineLevel="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="299" ht="11" customHeight="true" outlineLevel="3">
       <c r="B299" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="C299" s="11" t="n">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="300" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C299" s="16" t="n">
+        <v>5775</v>
+      </c>
+    </row>
+    <row r="300" ht="11" customHeight="true" outlineLevel="3">
       <c r="B300" s="15" t="s">
         <v>299</v>
       </c>
       <c r="C300" s="16" t="n">
-        <v>6958</v>
-      </c>
-    </row>
-    <row r="301" ht="22" customHeight="true" outlineLevel="3">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="301" ht="11" customHeight="true" outlineLevel="3">
       <c r="B301" s="15" t="s">
         <v>300</v>
       </c>
       <c r="C301" s="11" t="n">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="302" ht="22" customHeight="true" outlineLevel="3">
-      <c r="B302" s="15" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="302" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B302" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="C302" s="11" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="303" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C302" s="17" t="n">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="303" ht="11" customHeight="true" outlineLevel="3">
       <c r="B303" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="C303" s="16" t="n">
-        <v>5741</v>
-      </c>
-    </row>
-    <row r="304" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C303" s="11" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="304" ht="11" customHeight="true" outlineLevel="3">
       <c r="B304" s="15" t="s">
         <v>303</v>
       </c>
       <c r="C304" s="11" t="n">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="305" ht="22" customHeight="true" outlineLevel="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="305" ht="11" customHeight="true" outlineLevel="3">
       <c r="B305" s="15" t="s">
         <v>304</v>
       </c>
       <c r="C305" s="11" t="n">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="306" ht="11" customHeight="true" outlineLevel="3">
@@ -3816,15 +3852,15 @@
         <v>305</v>
       </c>
       <c r="C306" s="11" t="n">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="307" ht="11" customHeight="true" outlineLevel="3">
-      <c r="B307" s="15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="307" ht="11" customHeight="true" outlineLevel="2">
+      <c r="B307" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="C307" s="11" t="n">
-        <v>853</v>
+      <c r="C307" s="12" t="n">
+        <v>111323</v>
       </c>
     </row>
     <row r="308" ht="11" customHeight="true" outlineLevel="3">
@@ -3832,23 +3868,23 @@
         <v>307</v>
       </c>
       <c r="C308" s="11" t="n">
-        <v>65</v>
+        <v>220</v>
       </c>
     </row>
     <row r="309" ht="11" customHeight="true" outlineLevel="3">
       <c r="B309" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="C309" s="16" t="n">
-        <v>1217</v>
+      <c r="C309" s="11" t="n">
+        <v>253</v>
       </c>
     </row>
     <row r="310" ht="22" customHeight="true" outlineLevel="3">
       <c r="B310" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="C310" s="16" t="n">
-        <v>1135</v>
+      <c r="C310" s="11" t="n">
+        <v>538</v>
       </c>
     </row>
     <row r="311" ht="22" customHeight="true" outlineLevel="3">
@@ -3856,7 +3892,7 @@
         <v>310</v>
       </c>
       <c r="C311" s="11" t="n">
-        <v>15</v>
+        <v>364</v>
       </c>
     </row>
     <row r="312" ht="22" customHeight="true" outlineLevel="3">
@@ -3864,7 +3900,7 @@
         <v>311</v>
       </c>
       <c r="C312" s="16" t="n">
-        <v>1886</v>
+        <v>6704</v>
       </c>
     </row>
     <row r="313" ht="22" customHeight="true" outlineLevel="3">
@@ -3872,31 +3908,31 @@
         <v>312</v>
       </c>
       <c r="C313" s="11" t="n">
-        <v>122</v>
+        <v>615</v>
       </c>
     </row>
     <row r="314" ht="22" customHeight="true" outlineLevel="3">
       <c r="B314" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C314" s="16" t="n">
-        <v>4841</v>
+      <c r="C314" s="11" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="315" ht="22" customHeight="true" outlineLevel="3">
       <c r="B315" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="C315" s="11" t="n">
-        <v>659</v>
+      <c r="C315" s="16" t="n">
+        <v>5376</v>
       </c>
     </row>
     <row r="316" ht="22" customHeight="true" outlineLevel="3">
       <c r="B316" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="C316" s="16" t="n">
-        <v>2052</v>
+      <c r="C316" s="11" t="n">
+        <v>298</v>
       </c>
     </row>
     <row r="317" ht="22" customHeight="true" outlineLevel="3">
@@ -3904,47 +3940,47 @@
         <v>316</v>
       </c>
       <c r="C317" s="11" t="n">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="318" ht="22" customHeight="true" outlineLevel="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="318" ht="11" customHeight="true" outlineLevel="3">
       <c r="B318" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="C318" s="16" t="n">
-        <v>4006</v>
-      </c>
-    </row>
-    <row r="319" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C318" s="11" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="319" ht="11" customHeight="true" outlineLevel="3">
       <c r="B319" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C319" s="11" t="n">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="320" ht="22" customHeight="true" outlineLevel="3">
+      <c r="C319" s="16" t="n">
+        <v>3832</v>
+      </c>
+    </row>
+    <row r="320" ht="11" customHeight="true" outlineLevel="3">
       <c r="B320" s="15" t="s">
         <v>319</v>
       </c>
       <c r="C320" s="11" t="n">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="321" ht="22" customHeight="true" outlineLevel="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="321" ht="11" customHeight="true" outlineLevel="3">
       <c r="B321" s="15" t="s">
         <v>320</v>
       </c>
       <c r="C321" s="16" t="n">
-        <v>13635</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="322" ht="22" customHeight="true" outlineLevel="3">
       <c r="B322" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="C322" s="11" t="n">
-        <v>148</v>
+      <c r="C322" s="16" t="n">
+        <v>1110</v>
       </c>
     </row>
     <row r="323" ht="22" customHeight="true" outlineLevel="3">
@@ -3952,15 +3988,15 @@
         <v>322</v>
       </c>
       <c r="C323" s="11" t="n">
-        <v>294</v>
+        <v>3</v>
       </c>
     </row>
     <row r="324" ht="22" customHeight="true" outlineLevel="3">
       <c r="B324" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="C324" s="11" t="n">
-        <v>9</v>
+      <c r="C324" s="16" t="n">
+        <v>1873</v>
       </c>
     </row>
     <row r="325" ht="22" customHeight="true" outlineLevel="3">
@@ -3968,15 +4004,15 @@
         <v>324</v>
       </c>
       <c r="C325" s="11" t="n">
-        <v>345</v>
+        <v>78</v>
       </c>
     </row>
     <row r="326" ht="22" customHeight="true" outlineLevel="3">
       <c r="B326" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="C326" s="11" t="n">
-        <v>367</v>
+      <c r="C326" s="16" t="n">
+        <v>4420</v>
       </c>
     </row>
     <row r="327" ht="22" customHeight="true" outlineLevel="3">
@@ -3984,15 +4020,15 @@
         <v>326</v>
       </c>
       <c r="C327" s="11" t="n">
-        <v>772</v>
+        <v>649</v>
       </c>
     </row>
     <row r="328" ht="22" customHeight="true" outlineLevel="3">
       <c r="B328" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="C328" s="11" t="n">
-        <v>174</v>
+      <c r="C328" s="16" t="n">
+        <v>2040</v>
       </c>
     </row>
     <row r="329" ht="22" customHeight="true" outlineLevel="3">
@@ -4000,55 +4036,55 @@
         <v>328</v>
       </c>
       <c r="C329" s="11" t="n">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="330" ht="11" customHeight="true" outlineLevel="3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="330" ht="22" customHeight="true" outlineLevel="3">
       <c r="B330" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="C330" s="11" t="n">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="331" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C330" s="16" t="n">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="331" ht="22" customHeight="true" outlineLevel="3">
       <c r="B331" s="15" t="s">
         <v>330</v>
       </c>
       <c r="C331" s="11" t="n">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="332" ht="11" customHeight="true" outlineLevel="3">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="332" ht="22" customHeight="true" outlineLevel="3">
       <c r="B332" s="15" t="s">
         <v>331</v>
       </c>
       <c r="C332" s="11" t="n">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="333" ht="11" customHeight="true" outlineLevel="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="333" ht="22" customHeight="true" outlineLevel="3">
       <c r="B333" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="C333" s="11" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="334" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C333" s="16" t="n">
+        <v>13452</v>
+      </c>
+    </row>
+    <row r="334" ht="22" customHeight="true" outlineLevel="3">
       <c r="B334" s="15" t="s">
         <v>333</v>
       </c>
       <c r="C334" s="11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="335" ht="11" customHeight="true" outlineLevel="3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="335" ht="22" customHeight="true" outlineLevel="3">
       <c r="B335" s="15" t="s">
         <v>334</v>
       </c>
       <c r="C335" s="11" t="n">
-        <v>967</v>
+        <v>174</v>
       </c>
     </row>
     <row r="336" ht="22" customHeight="true" outlineLevel="3">
@@ -4056,15 +4092,15 @@
         <v>335</v>
       </c>
       <c r="C336" s="11" t="n">
-        <v>661</v>
+        <v>9</v>
       </c>
     </row>
     <row r="337" ht="22" customHeight="true" outlineLevel="3">
       <c r="B337" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="C337" s="11" t="n">
-        <v>112</v>
+      <c r="C337" s="16" t="n">
+        <v>1618</v>
       </c>
     </row>
     <row r="338" ht="22" customHeight="true" outlineLevel="3">
@@ -4072,7 +4108,7 @@
         <v>337</v>
       </c>
       <c r="C338" s="11" t="n">
-        <v>155</v>
+        <v>345</v>
       </c>
     </row>
     <row r="339" ht="22" customHeight="true" outlineLevel="3">
@@ -4080,15 +4116,15 @@
         <v>338</v>
       </c>
       <c r="C339" s="11" t="n">
-        <v>88</v>
+        <v>218</v>
       </c>
     </row>
     <row r="340" ht="22" customHeight="true" outlineLevel="3">
       <c r="B340" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C340" s="16" t="n">
-        <v>3327</v>
+      <c r="C340" s="11" t="n">
+        <v>159</v>
       </c>
     </row>
     <row r="341" ht="22" customHeight="true" outlineLevel="3">
@@ -4096,15 +4132,15 @@
         <v>340</v>
       </c>
       <c r="C341" s="11" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="342" ht="22" customHeight="true" outlineLevel="3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="342" ht="11" customHeight="true" outlineLevel="3">
       <c r="B342" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="C342" s="16" t="n">
-        <v>4033</v>
+      <c r="C342" s="11" t="n">
+        <v>145</v>
       </c>
     </row>
     <row r="343" ht="11" customHeight="true" outlineLevel="3">
@@ -4112,15 +4148,15 @@
         <v>342</v>
       </c>
       <c r="C343" s="11" t="n">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="344" ht="22" customHeight="true" outlineLevel="3">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="344" ht="11" customHeight="true" outlineLevel="3">
       <c r="B344" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="C344" s="16" t="n">
-        <v>3088</v>
+      <c r="C344" s="11" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="345" ht="11" customHeight="true" outlineLevel="3">
@@ -4128,7 +4164,7 @@
         <v>344</v>
       </c>
       <c r="C345" s="11" t="n">
-        <v>652</v>
+        <v>65</v>
       </c>
     </row>
     <row r="346" ht="11" customHeight="true" outlineLevel="3">
@@ -4136,39 +4172,39 @@
         <v>345</v>
       </c>
       <c r="C346" s="11" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="347" ht="22" customHeight="true" outlineLevel="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="347" ht="11" customHeight="true" outlineLevel="3">
       <c r="B347" s="15" t="s">
         <v>346</v>
       </c>
       <c r="C347" s="11" t="n">
-        <v>102</v>
+        <v>953</v>
       </c>
     </row>
     <row r="348" ht="22" customHeight="true" outlineLevel="3">
       <c r="B348" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="C348" s="16" t="n">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="349" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C348" s="11" t="n">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="349" ht="22" customHeight="true" outlineLevel="3">
       <c r="B349" s="15" t="s">
         <v>348</v>
       </c>
       <c r="C349" s="11" t="n">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="350" ht="11" customHeight="true" outlineLevel="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="350" ht="22" customHeight="true" outlineLevel="3">
       <c r="B350" s="15" t="s">
         <v>349</v>
       </c>
       <c r="C350" s="11" t="n">
-        <v>80</v>
+        <v>145</v>
       </c>
     </row>
     <row r="351" ht="22" customHeight="true" outlineLevel="3">
@@ -4176,23 +4212,23 @@
         <v>350</v>
       </c>
       <c r="C351" s="11" t="n">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="352" ht="22" customHeight="true" outlineLevel="3">
       <c r="B352" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="C352" s="11" t="n">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="353" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C352" s="16" t="n">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="353" ht="22" customHeight="true" outlineLevel="3">
       <c r="B353" s="15" t="s">
         <v>352</v>
       </c>
       <c r="C353" s="11" t="n">
-        <v>599</v>
+        <v>107</v>
       </c>
     </row>
     <row r="354" ht="22" customHeight="true" outlineLevel="3">
@@ -4200,23 +4236,23 @@
         <v>353</v>
       </c>
       <c r="C354" s="16" t="n">
-        <v>1030</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="355" ht="11" customHeight="true" outlineLevel="3">
       <c r="B355" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="C355" s="16" t="n">
-        <v>2922</v>
-      </c>
-    </row>
-    <row r="356" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C355" s="11" t="n">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="356" ht="22" customHeight="true" outlineLevel="3">
       <c r="B356" s="15" t="s">
         <v>355</v>
       </c>
       <c r="C356" s="16" t="n">
-        <v>1991</v>
+        <v>3014</v>
       </c>
     </row>
     <row r="357" ht="11" customHeight="true" outlineLevel="3">
@@ -4224,7 +4260,7 @@
         <v>356</v>
       </c>
       <c r="C357" s="11" t="n">
-        <v>898</v>
+        <v>639</v>
       </c>
     </row>
     <row r="358" ht="11" customHeight="true" outlineLevel="3">
@@ -4232,23 +4268,23 @@
         <v>357</v>
       </c>
       <c r="C358" s="11" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="359" ht="11" customHeight="true" outlineLevel="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="359" ht="22" customHeight="true" outlineLevel="3">
       <c r="B359" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="C359" s="16" t="n">
-        <v>2934</v>
+      <c r="C359" s="11" t="n">
+        <v>102</v>
       </c>
     </row>
     <row r="360" ht="22" customHeight="true" outlineLevel="3">
       <c r="B360" s="15" t="s">
         <v>359</v>
       </c>
-      <c r="C360" s="11" t="n">
-        <v>639</v>
+      <c r="C360" s="16" t="n">
+        <v>1592</v>
       </c>
     </row>
     <row r="361" ht="11" customHeight="true" outlineLevel="3">
@@ -4256,63 +4292,63 @@
         <v>360</v>
       </c>
       <c r="C361" s="11" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="362" ht="22" customHeight="true" outlineLevel="3">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="362" ht="11" customHeight="true" outlineLevel="3">
       <c r="B362" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="C362" s="16" t="n">
-        <v>4271</v>
-      </c>
-    </row>
-    <row r="363" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C362" s="11" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="363" ht="22" customHeight="true" outlineLevel="3">
       <c r="B363" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="C363" s="16" t="n">
-        <v>2376</v>
-      </c>
-    </row>
-    <row r="364" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C363" s="11" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="364" ht="22" customHeight="true" outlineLevel="3">
       <c r="B364" s="15" t="s">
         <v>363</v>
       </c>
       <c r="C364" s="11" t="n">
-        <v>522</v>
+        <v>167</v>
       </c>
     </row>
     <row r="365" ht="11" customHeight="true" outlineLevel="3">
       <c r="B365" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="C365" s="16" t="n">
-        <v>3993</v>
-      </c>
-    </row>
-    <row r="366" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C365" s="11" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="366" ht="22" customHeight="true" outlineLevel="3">
       <c r="B366" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="C366" s="16" t="n">
-        <v>5124</v>
+      <c r="C366" s="11" t="n">
+        <v>938</v>
       </c>
     </row>
     <row r="367" ht="11" customHeight="true" outlineLevel="3">
       <c r="B367" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="C367" s="11" t="n">
-        <v>65</v>
+      <c r="C367" s="16" t="n">
+        <v>2621</v>
       </c>
     </row>
     <row r="368" ht="11" customHeight="true" outlineLevel="3">
       <c r="B368" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="C368" s="11" t="n">
-        <v>266</v>
+      <c r="C368" s="16" t="n">
+        <v>1972</v>
       </c>
     </row>
     <row r="369" ht="11" customHeight="true" outlineLevel="3">
@@ -4320,7 +4356,7 @@
         <v>368</v>
       </c>
       <c r="C369" s="11" t="n">
-        <v>525</v>
+        <v>658</v>
       </c>
     </row>
     <row r="370" ht="11" customHeight="true" outlineLevel="3">
@@ -4328,46 +4364,142 @@
         <v>369</v>
       </c>
       <c r="C370" s="11" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="371" ht="11" customHeight="true" outlineLevel="3">
       <c r="B371" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="C371" s="11" t="n">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="372" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C371" s="16" t="n">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="372" ht="22" customHeight="true" outlineLevel="3">
       <c r="B372" s="15" t="s">
         <v>371</v>
       </c>
       <c r="C372" s="11" t="n">
-        <v>673</v>
+        <v>439</v>
       </c>
     </row>
     <row r="373" ht="11" customHeight="true" outlineLevel="3">
       <c r="B373" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="C373" s="16" t="n">
-        <v>5637</v>
-      </c>
-    </row>
-    <row r="374" ht="11" customHeight="true" outlineLevel="3">
+      <c r="C373" s="11" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="374" ht="22" customHeight="true" outlineLevel="3">
       <c r="B374" s="15" t="s">
         <v>373</v>
       </c>
       <c r="C374" s="16" t="n">
-        <v>12647</v>
-      </c>
-    </row>
-    <row r="375" ht="22" customHeight="true" outlineLevel="3">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="375" ht="11" customHeight="true" outlineLevel="3">
       <c r="B375" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="C375" s="11" t="n">
+      <c r="C375" s="16" t="n">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="376" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B376" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="C376" s="11" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="377" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B377" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="C377" s="16" t="n">
+        <v>3542</v>
+      </c>
+    </row>
+    <row r="378" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B378" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="C378" s="16" t="n">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="379" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B379" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="C379" s="11" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="380" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B380" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="C380" s="11" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="381" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B381" s="15" t="s">
+        <v>380</v>
+      </c>
+      <c r="C381" s="11" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="382" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B382" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="C382" s="11" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="383" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B383" s="15" t="s">
+        <v>382</v>
+      </c>
+      <c r="C383" s="11" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="384" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B384" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="C384" s="11" t="n">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="385" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B385" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="C385" s="16" t="n">
+        <v>5522</v>
+      </c>
+    </row>
+    <row r="386" ht="11" customHeight="true" outlineLevel="3">
+      <c r="B386" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="C386" s="16" t="n">
+        <v>12531</v>
+      </c>
+    </row>
+    <row r="387" ht="22" customHeight="true" outlineLevel="3">
+      <c r="B387" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="C387" s="11" t="n">
         <v>360</v>
       </c>
     </row>

</xml_diff>